<commit_message>
implemented no coupling condition
</commit_message>
<xml_diff>
--- a/simulated_data/dyads_simulated/cond1_drifting_coupling/HRV_B.xlsx
+++ b/simulated_data/dyads_simulated/cond1_drifting_coupling/HRV_B.xlsx
@@ -1030,2892 +1030,2892 @@
     </row>
     <row r="122">
       <c r="A122" t="n">
-        <v>633.0888192498918</v>
+        <v>633.0888192510855</v>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="n">
-        <v>718.4549306665389</v>
+        <v>718.4549306421388</v>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="n">
-        <v>762.4958967512327</v>
+        <v>762.4958835192075</v>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="n">
-        <v>767.6787034188948</v>
+        <v>767.6838065810472</v>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="n">
-        <v>720.1940296835829</v>
+        <v>720.2156628213885</v>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="n">
-        <v>716.8846621452047</v>
+        <v>716.8982640294672</v>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="n">
-        <v>718.8370872916039</v>
+        <v>718.8301137592532</v>
       </c>
     </row>
     <row r="129">
       <c r="A129" t="n">
-        <v>739.2039538662516</v>
+        <v>739.1988175491377</v>
       </c>
     </row>
     <row r="130">
       <c r="A130" t="n">
-        <v>791.0012772773598</v>
+        <v>790.8727742255479</v>
       </c>
     </row>
     <row r="131">
       <c r="A131" t="n">
-        <v>776.3950673177504</v>
+        <v>776.0374789777131</v>
       </c>
     </row>
     <row r="132">
       <c r="A132" t="n">
-        <v>782.9772750402668</v>
+        <v>782.7992550764975</v>
       </c>
     </row>
     <row r="133">
       <c r="A133" t="n">
-        <v>740.8692733692277</v>
+        <v>741.1741090398039</v>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="n">
-        <v>747.3785275919056</v>
+        <v>747.6226499435796</v>
       </c>
     </row>
     <row r="135">
       <c r="A135" t="n">
-        <v>717.064841955974</v>
+        <v>717.647538108622</v>
       </c>
     </row>
     <row r="136">
       <c r="A136" t="n">
-        <v>658.988466945658</v>
+        <v>659.6914409838632</v>
       </c>
     </row>
     <row r="137">
       <c r="A137" t="n">
-        <v>663.5025446567511</v>
+        <v>663.465328057697</v>
       </c>
     </row>
     <row r="138">
       <c r="A138" t="n">
-        <v>689.7159182943398</v>
+        <v>688.8492373093413</v>
       </c>
     </row>
     <row r="139">
       <c r="A139" t="n">
-        <v>735.3450969682456</v>
+        <v>733.6290008814075</v>
       </c>
     </row>
     <row r="140">
       <c r="A140" t="n">
-        <v>667.0123361719504</v>
+        <v>665.0024946938231</v>
       </c>
     </row>
     <row r="141">
       <c r="A141" t="n">
-        <v>565.9622923617036</v>
+        <v>564.3533104000511</v>
       </c>
     </row>
     <row r="142">
       <c r="A142" t="n">
-        <v>503.7445441264481</v>
+        <v>502.1346907630146</v>
       </c>
     </row>
     <row r="143">
       <c r="A143" t="n">
-        <v>502.8606766145032</v>
+        <v>501.2591713878152</v>
       </c>
     </row>
     <row r="144">
       <c r="A144" t="n">
-        <v>502.5449419694183</v>
+        <v>500.9632638842589</v>
       </c>
     </row>
     <row r="145">
       <c r="A145" t="n">
-        <v>576.2900490722842</v>
+        <v>573.0711153411363</v>
       </c>
     </row>
     <row r="146">
       <c r="A146" t="n">
-        <v>696.6519475996051</v>
+        <v>693.7258059800371</v>
       </c>
     </row>
     <row r="147">
       <c r="A147" t="n">
-        <v>764.1275756337507</v>
+        <v>763.4208402837714</v>
       </c>
     </row>
     <row r="148">
       <c r="A148" t="n">
-        <v>775.4318435380725</v>
+        <v>776.5633391446727</v>
       </c>
     </row>
     <row r="149">
       <c r="A149" t="n">
-        <v>750.775592751026</v>
+        <v>752.7294521191976</v>
       </c>
     </row>
     <row r="150">
       <c r="A150" t="n">
-        <v>647.200856989457</v>
+        <v>649.0496910402754</v>
       </c>
     </row>
     <row r="151">
       <c r="A151" t="n">
-        <v>595.7913660317899</v>
+        <v>596.248064795347</v>
       </c>
     </row>
     <row r="152">
       <c r="A152" t="n">
-        <v>585.5970617264319</v>
+        <v>583.0564976404702</v>
       </c>
     </row>
     <row r="153">
       <c r="A153" t="n">
-        <v>615.9938079355953</v>
+        <v>610.8887234734794</v>
       </c>
     </row>
     <row r="154">
       <c r="A154" t="n">
-        <v>639.2220613321768</v>
+        <v>635.6269546011788</v>
       </c>
     </row>
     <row r="155">
       <c r="A155" t="n">
-        <v>564.0966415583364</v>
+        <v>561.2821310918434</v>
       </c>
     </row>
     <row r="156">
       <c r="A156" t="n">
-        <v>582.0967555782772</v>
+        <v>574.0191877714693</v>
       </c>
     </row>
     <row r="157">
       <c r="A157" t="n">
-        <v>606.0598082315778</v>
+        <v>593.5289345296155</v>
       </c>
     </row>
     <row r="158">
       <c r="A158" t="n">
-        <v>636.1850365237842</v>
+        <v>622.2111830307853</v>
       </c>
     </row>
     <row r="159">
       <c r="A159" t="n">
-        <v>724.3602400455558</v>
+        <v>710.1770424344096</v>
       </c>
     </row>
     <row r="160">
       <c r="A160" t="n">
-        <v>743.9418801920681</v>
+        <v>741.3708234748384</v>
       </c>
     </row>
     <row r="161">
       <c r="A161" t="n">
-        <v>721.1757206900131</v>
+        <v>716.759462511277</v>
       </c>
     </row>
     <row r="162">
       <c r="A162" t="n">
-        <v>725.9089214003751</v>
+        <v>727.8361816513268</v>
       </c>
     </row>
     <row r="163">
       <c r="A163" t="n">
-        <v>630.7088748884127</v>
+        <v>631.6000859504953</v>
       </c>
     </row>
     <row r="164">
       <c r="A164" t="n">
-        <v>573.8251940845629</v>
+        <v>566.7645837428097</v>
       </c>
     </row>
     <row r="165">
       <c r="A165" t="n">
-        <v>629.6487584534276</v>
+        <v>607.7228922316635</v>
       </c>
     </row>
     <row r="166">
       <c r="A166" t="n">
-        <v>667.138683740049</v>
+        <v>656.973872934941</v>
       </c>
     </row>
     <row r="167">
       <c r="A167" t="n">
-        <v>671.9456457901032</v>
+        <v>670.8918125135455</v>
       </c>
     </row>
     <row r="168">
       <c r="A168" t="n">
-        <v>707.737831885737</v>
+        <v>703.5723800171212</v>
       </c>
     </row>
     <row r="169">
       <c r="A169" t="n">
-        <v>697.9927161764721</v>
+        <v>707.5245744188123</v>
       </c>
     </row>
     <row r="170">
       <c r="A170" t="n">
-        <v>614.1167522519453</v>
+        <v>622.9273398591886</v>
       </c>
     </row>
     <row r="171">
       <c r="A171" t="n">
-        <v>596.8150828506396</v>
+        <v>596.5574459560372</v>
       </c>
     </row>
     <row r="172">
       <c r="A172" t="n">
-        <v>651.153669968906</v>
+        <v>645.3016851321252</v>
       </c>
     </row>
     <row r="173">
       <c r="A173" t="n">
-        <v>643.3847686006686</v>
+        <v>631.5014549155364</v>
       </c>
     </row>
     <row r="174">
       <c r="A174" t="n">
-        <v>603.4625839502183</v>
+        <v>585.5198384110736</v>
       </c>
     </row>
     <row r="175">
       <c r="A175" t="n">
-        <v>563.0153264276316</v>
+        <v>550.1841626471702</v>
       </c>
     </row>
     <row r="176">
       <c r="A176" t="n">
-        <v>519.9417125584631</v>
+        <v>528.1811184708829</v>
       </c>
     </row>
     <row r="177">
       <c r="A177" t="n">
-        <v>486.3231867113456</v>
+        <v>494.8320248933413</v>
       </c>
     </row>
     <row r="178">
       <c r="A178" t="n">
-        <v>494.1317180637697</v>
+        <v>499.0667075503978</v>
       </c>
     </row>
     <row r="179">
       <c r="A179" t="n">
-        <v>545.8135840002143</v>
+        <v>529.2414148141091</v>
       </c>
     </row>
     <row r="180">
       <c r="A180" t="n">
-        <v>632.62831566567</v>
+        <v>619.7927278431195</v>
       </c>
     </row>
     <row r="181">
       <c r="A181" t="n">
-        <v>730.0650270047839</v>
+        <v>722.6444807352408</v>
       </c>
     </row>
     <row r="182">
       <c r="A182" t="n">
-        <v>810.1251124582518</v>
+        <v>804.2332317363332</v>
       </c>
     </row>
     <row r="183">
       <c r="A183" t="n">
-        <v>784.2806684374324</v>
+        <v>788.6309801185689</v>
       </c>
     </row>
     <row r="184">
       <c r="A184" t="n">
-        <v>728.9587771264365</v>
+        <v>726.0765190749936</v>
       </c>
     </row>
     <row r="185">
       <c r="A185" t="n">
-        <v>699.7113974912139</v>
+        <v>692.949261417084</v>
       </c>
     </row>
     <row r="186">
       <c r="A186" t="n">
-        <v>668.2594483445712</v>
+        <v>671.6664468324325</v>
       </c>
     </row>
     <row r="187">
       <c r="A187" t="n">
-        <v>543.9563357373061</v>
+        <v>569.8870113214412</v>
       </c>
     </row>
     <row r="188">
       <c r="A188" t="n">
-        <v>460.911224913346</v>
+        <v>482.1992541288012</v>
       </c>
     </row>
     <row r="189">
       <c r="A189" t="n">
-        <v>451.150609721239</v>
+        <v>447.1738877230962</v>
       </c>
     </row>
     <row r="190">
       <c r="A190" t="n">
-        <v>530.8826934714972</v>
+        <v>502.3827862482761</v>
       </c>
     </row>
     <row r="191">
       <c r="A191" t="n">
-        <v>621.2615383098381</v>
+        <v>584.0211793569665</v>
       </c>
     </row>
     <row r="192">
       <c r="A192" t="n">
-        <v>676.9118820212867</v>
+        <v>659.4199896307487</v>
       </c>
     </row>
     <row r="193">
       <c r="A193" t="n">
-        <v>666.8991730897318</v>
+        <v>647.1079540320233</v>
       </c>
     </row>
     <row r="194">
       <c r="A194" t="n">
-        <v>664.6174938110647</v>
+        <v>636.7510074386189</v>
       </c>
     </row>
     <row r="195">
       <c r="A195" t="n">
-        <v>722.4106077902519</v>
+        <v>668.6046644349659</v>
       </c>
     </row>
     <row r="196">
       <c r="A196" t="n">
-        <v>707.2169256578889</v>
+        <v>691.7769546205506</v>
       </c>
     </row>
     <row r="197">
       <c r="A197" t="n">
-        <v>688.1258520050153</v>
+        <v>649.0703721924973</v>
       </c>
     </row>
     <row r="198">
       <c r="A198" t="n">
-        <v>629.4033721401036</v>
+        <v>636.5381485298798</v>
       </c>
     </row>
     <row r="199">
       <c r="A199" t="n">
-        <v>580.9839543553181</v>
+        <v>593.0885685760359</v>
       </c>
     </row>
     <row r="200">
       <c r="A200" t="n">
-        <v>549.3166882637439</v>
+        <v>553.2234834875993</v>
       </c>
     </row>
     <row r="201">
       <c r="A201" t="n">
-        <v>542.4202098968891</v>
+        <v>515.7119590195549</v>
       </c>
     </row>
     <row r="202">
       <c r="A202" t="n">
-        <v>562.4468338413919</v>
+        <v>550.3284678675726</v>
       </c>
     </row>
     <row r="203">
       <c r="A203" t="n">
-        <v>562.1346382687449</v>
+        <v>557.1042051959267</v>
       </c>
     </row>
     <row r="204">
       <c r="A204" t="n">
-        <v>548.1259835832333</v>
+        <v>566.2599649520388</v>
       </c>
     </row>
     <row r="205">
       <c r="A205" t="n">
-        <v>563.9201047736009</v>
+        <v>541.4225783854363</v>
       </c>
     </row>
     <row r="206">
       <c r="A206" t="n">
-        <v>622.2376852358309</v>
+        <v>570.252216336371</v>
       </c>
     </row>
     <row r="207">
       <c r="A207" t="n">
-        <v>661.1872577449986</v>
+        <v>629.3360258754461</v>
       </c>
     </row>
     <row r="208">
       <c r="A208" t="n">
-        <v>643.5080849424253</v>
+        <v>651.3822002788032</v>
       </c>
     </row>
     <row r="209">
       <c r="A209" t="n">
-        <v>607.5644081379323</v>
+        <v>643.6258460793027</v>
       </c>
     </row>
     <row r="210">
       <c r="A210" t="n">
-        <v>581.9588912432323</v>
+        <v>596.5870658831136</v>
       </c>
     </row>
     <row r="211">
       <c r="A211" t="n">
-        <v>588.2356122877752</v>
+        <v>583.8799456498407</v>
       </c>
     </row>
     <row r="212">
       <c r="A212" t="n">
-        <v>567.4409970244483</v>
+        <v>589.9269294930036</v>
       </c>
     </row>
     <row r="213">
       <c r="A213" t="n">
-        <v>508.7276362667694</v>
+        <v>553.6066106375017</v>
       </c>
     </row>
     <row r="214">
       <c r="A214" t="n">
-        <v>505.4900464411105</v>
+        <v>519.2492243236586</v>
       </c>
     </row>
     <row r="215">
       <c r="A215" t="n">
-        <v>503.2330248448602</v>
+        <v>512.6584688119351</v>
       </c>
     </row>
     <row r="216">
       <c r="A216" t="n">
-        <v>498.2261413070148</v>
+        <v>507.6577811122149</v>
       </c>
     </row>
     <row r="217">
       <c r="A217" t="n">
-        <v>498.5434232412445</v>
+        <v>507.3214477037311</v>
       </c>
     </row>
     <row r="218">
       <c r="A218" t="n">
-        <v>494.6140174846505</v>
+        <v>504.0153013162296</v>
       </c>
     </row>
     <row r="219">
       <c r="A219" t="n">
-        <v>539.6087187381795</v>
+        <v>516.106717754667</v>
       </c>
     </row>
     <row r="220">
       <c r="A220" t="n">
-        <v>526.4610286822631</v>
+        <v>541.6069829348942</v>
       </c>
     </row>
     <row r="221">
       <c r="A221" t="n">
-        <v>555.5969336895146</v>
+        <v>525.0014022967662</v>
       </c>
     </row>
     <row r="222">
       <c r="A222" t="n">
-        <v>561.067190191693</v>
+        <v>529.1767241104992</v>
       </c>
     </row>
     <row r="223">
       <c r="A223" t="n">
-        <v>577.9503015890839</v>
+        <v>529.682936443038</v>
       </c>
     </row>
     <row r="224">
       <c r="A224" t="n">
-        <v>608.6026892993459</v>
+        <v>549.5825869663804</v>
       </c>
     </row>
     <row r="225">
       <c r="A225" t="n">
-        <v>586.8397396056366</v>
+        <v>574.7430708496211</v>
       </c>
     </row>
     <row r="226">
       <c r="A226" t="n">
-        <v>596.589290204804</v>
+        <v>584.4222886809405</v>
       </c>
     </row>
     <row r="227">
       <c r="A227" t="n">
-        <v>653.722463725245</v>
+        <v>612.272675758561</v>
       </c>
     </row>
     <row r="228">
       <c r="A228" t="n">
-        <v>610.1751661987578</v>
+        <v>670.6660863170839</v>
       </c>
     </row>
     <row r="229">
       <c r="A229" t="n">
-        <v>592.3357540667098</v>
+        <v>603.0828751125625</v>
       </c>
     </row>
     <row r="230">
       <c r="A230" t="n">
-        <v>597.3683143831465</v>
+        <v>583.7481780706639</v>
       </c>
     </row>
     <row r="231">
       <c r="A231" t="n">
-        <v>628.7550991609692</v>
+        <v>585.7705718848365</v>
       </c>
     </row>
     <row r="232">
       <c r="A232" t="n">
-        <v>571.508803228113</v>
+        <v>610.5205720414233</v>
       </c>
     </row>
     <row r="233">
       <c r="A233" t="n">
-        <v>562.8410241286019</v>
+        <v>544.1739815764208</v>
       </c>
     </row>
     <row r="234">
       <c r="A234" t="n">
-        <v>492.3854375629162</v>
+        <v>537.2582250035975</v>
       </c>
     </row>
     <row r="235">
       <c r="A235" t="n">
-        <v>489.2239757591597</v>
+        <v>492.4124590332895</v>
       </c>
     </row>
     <row r="236">
       <c r="A236" t="n">
-        <v>488.1958432870306</v>
+        <v>509.7320517762682</v>
       </c>
     </row>
     <row r="237">
       <c r="A237" t="n">
-        <v>466.2771919530542</v>
+        <v>505.312455236691</v>
       </c>
     </row>
     <row r="238">
       <c r="A238" t="n">
-        <v>471.5954854093809</v>
+        <v>477.0469133485449</v>
       </c>
     </row>
     <row r="239">
       <c r="A239" t="n">
-        <v>541.8561183197426</v>
+        <v>492.7688162956088</v>
       </c>
     </row>
     <row r="240">
       <c r="A240" t="n">
-        <v>581.8054814938307</v>
+        <v>560.8031388845518</v>
       </c>
     </row>
     <row r="241">
       <c r="A241" t="n">
-        <v>539.3022950287047</v>
+        <v>564.2828881167361</v>
       </c>
     </row>
     <row r="242">
       <c r="A242" t="n">
-        <v>504.6997369585142</v>
+        <v>519.1415811503646</v>
       </c>
     </row>
     <row r="243">
       <c r="A243" t="n">
-        <v>489.5563929015907</v>
+        <v>494.3416967819871</v>
       </c>
     </row>
     <row r="244">
       <c r="A244" t="n">
-        <v>548.1734406195642</v>
+        <v>497.9268777557877</v>
       </c>
     </row>
     <row r="245">
       <c r="A245" t="n">
-        <v>690.0263517192968</v>
+        <v>567.4476377976987</v>
       </c>
     </row>
     <row r="246">
       <c r="A246" t="n">
-        <v>798.4307063699134</v>
+        <v>715.3653296300604</v>
       </c>
     </row>
     <row r="247">
       <c r="A247" t="n">
-        <v>749.5481635510259</v>
+        <v>806.3572681717233</v>
       </c>
     </row>
     <row r="248">
       <c r="A248" t="n">
-        <v>737.8253168475055</v>
+        <v>755.7919232559414</v>
       </c>
     </row>
     <row r="249">
       <c r="A249" t="n">
-        <v>694.714950757259</v>
+        <v>752.9935807902746</v>
       </c>
     </row>
     <row r="250">
       <c r="A250" t="n">
-        <v>577.8907933063238</v>
+        <v>675.471800469893</v>
       </c>
     </row>
     <row r="251">
       <c r="A251" t="n">
-        <v>475.1752484714871</v>
+        <v>561.1602861247036</v>
       </c>
     </row>
     <row r="252">
       <c r="A252" t="n">
-        <v>432.3642577666931</v>
+        <v>471.1742914407182</v>
       </c>
     </row>
     <row r="253">
       <c r="A253" t="n">
-        <v>448.3462090267665</v>
+        <v>435.8008754138325</v>
       </c>
     </row>
     <row r="254">
       <c r="A254" t="n">
-        <v>539.7399032050032</v>
+        <v>460.4555513624859</v>
       </c>
     </row>
     <row r="255">
       <c r="A255" t="n">
-        <v>547.6111001932509</v>
+        <v>520.2129125406714</v>
       </c>
     </row>
     <row r="256">
       <c r="A256" t="n">
-        <v>562.6698270093016</v>
+        <v>528.3704132259288</v>
       </c>
     </row>
     <row r="257">
       <c r="A257" t="n">
-        <v>640.5446566419073</v>
+        <v>551.6661603559783</v>
       </c>
     </row>
     <row r="258">
       <c r="A258" t="n">
-        <v>660.3859214120007</v>
+        <v>648.0409144227792</v>
       </c>
     </row>
     <row r="259">
       <c r="A259" t="n">
-        <v>599.5478677320705</v>
+        <v>677.2397864218078</v>
       </c>
     </row>
     <row r="260">
       <c r="A260" t="n">
-        <v>587.0907456429109</v>
+        <v>611.0827186537904</v>
       </c>
     </row>
     <row r="261">
       <c r="A261" t="n">
-        <v>624.3307144228254</v>
+        <v>607.3449697455828</v>
       </c>
     </row>
     <row r="262">
       <c r="A262" t="n">
-        <v>647.8027004926616</v>
+        <v>646.1727851286128</v>
       </c>
     </row>
     <row r="263">
       <c r="A263" t="n">
-        <v>670.6736277220386</v>
+        <v>669.9306953932762</v>
       </c>
     </row>
     <row r="264">
       <c r="A264" t="n">
-        <v>695.6141573906791</v>
+        <v>677.4951796623441</v>
       </c>
     </row>
     <row r="265">
       <c r="A265" t="n">
-        <v>718.5392335290715</v>
+        <v>707.1863424241087</v>
       </c>
     </row>
     <row r="266">
       <c r="A266" t="n">
-        <v>741.706059500018</v>
+        <v>725.0091745897578</v>
       </c>
     </row>
     <row r="267">
       <c r="A267" t="n">
-        <v>718.8430163201929</v>
+        <v>734.3515470034561</v>
       </c>
     </row>
     <row r="268">
       <c r="A268" t="n">
-        <v>647.7095937843842</v>
+        <v>683.64773729013</v>
       </c>
     </row>
     <row r="269">
       <c r="A269" t="n">
-        <v>555.3671802957467</v>
+        <v>600.3996420245983</v>
       </c>
     </row>
     <row r="270">
       <c r="A270" t="n">
-        <v>471.5317944180129</v>
+        <v>516.7503260987303</v>
       </c>
     </row>
     <row r="271">
       <c r="A271" t="n">
-        <v>459.6056840759104</v>
+        <v>440.2844656688671</v>
       </c>
     </row>
     <row r="272">
       <c r="A272" t="n">
-        <v>544.9622145649755</v>
+        <v>450.4241046509492</v>
       </c>
     </row>
     <row r="273">
       <c r="A273" t="n">
-        <v>609.1470913845853</v>
+        <v>560.5017580351159</v>
       </c>
     </row>
     <row r="274">
       <c r="A274" t="n">
-        <v>641.5489182344061</v>
+        <v>632.2197205024906</v>
       </c>
     </row>
     <row r="275">
       <c r="A275" t="n">
-        <v>685.8029574771365</v>
+        <v>664.934013886608</v>
       </c>
     </row>
     <row r="276">
       <c r="A276" t="n">
-        <v>733.9294988449296</v>
+        <v>707.9512872818441</v>
       </c>
     </row>
     <row r="277">
       <c r="A277" t="n">
-        <v>749.2027141635162</v>
+        <v>757.1970440574205</v>
       </c>
     </row>
     <row r="278">
       <c r="A278" t="n">
-        <v>739.0231943779497</v>
+        <v>756.622417104154</v>
       </c>
     </row>
     <row r="279">
       <c r="A279" t="n">
-        <v>727.9765671274561</v>
+        <v>729.7311110796159</v>
       </c>
     </row>
     <row r="280">
       <c r="A280" t="n">
-        <v>740.6128176635605</v>
+        <v>705.2940573808257</v>
       </c>
     </row>
     <row r="281">
       <c r="A281" t="n">
-        <v>816.668168639751</v>
+        <v>736.7425247158224</v>
       </c>
     </row>
     <row r="282">
       <c r="A282" t="n">
-        <v>838.7031822982181</v>
+        <v>819.6031221659155</v>
       </c>
     </row>
     <row r="283">
       <c r="A283" t="n">
-        <v>849.8371409258993</v>
+        <v>843.1312252715202</v>
       </c>
     </row>
     <row r="284">
       <c r="A284" t="n">
-        <v>807.8596645113976</v>
+        <v>844.258323183368</v>
       </c>
     </row>
     <row r="285">
       <c r="A285" t="n">
-        <v>750.7300263136756</v>
+        <v>801.742708229682</v>
       </c>
     </row>
     <row r="286">
       <c r="A286" t="n">
-        <v>654.4167219520602</v>
+        <v>720.580852453196</v>
       </c>
     </row>
     <row r="287">
       <c r="A287" t="n">
-        <v>677.5074084924029</v>
+        <v>648.302293903015</v>
       </c>
     </row>
     <row r="288">
       <c r="A288" t="n">
-        <v>696.8213327209014</v>
+        <v>668.8960142011524</v>
       </c>
     </row>
     <row r="289">
       <c r="A289" t="n">
-        <v>686.1578413077041</v>
+        <v>698.8376260736118</v>
       </c>
     </row>
     <row r="290">
       <c r="A290" t="n">
-        <v>695.1924875498037</v>
+        <v>687.2312741056419</v>
       </c>
     </row>
     <row r="291">
       <c r="A291" t="n">
-        <v>679.6851517668472</v>
+        <v>679.4327286351631</v>
       </c>
     </row>
     <row r="292">
       <c r="A292" t="n">
-        <v>698.2081212037485</v>
+        <v>670.7285736675033</v>
       </c>
     </row>
     <row r="293">
       <c r="A293" t="n">
-        <v>707.0568470783201</v>
+        <v>693.7998113098729</v>
       </c>
     </row>
     <row r="294">
       <c r="A294" t="n">
-        <v>722.3221324620113</v>
+        <v>704.6662871277647</v>
       </c>
     </row>
     <row r="295">
       <c r="A295" t="n">
-        <v>709.9707239550526</v>
+        <v>727.2598369008847</v>
       </c>
     </row>
     <row r="296">
       <c r="A296" t="n">
-        <v>697.5344341273342</v>
+        <v>718.3528841200655</v>
       </c>
     </row>
     <row r="297">
       <c r="A297" t="n">
-        <v>672.4720175101595</v>
+        <v>702.4823550241877</v>
       </c>
     </row>
     <row r="298">
       <c r="A298" t="n">
-        <v>684.7519278938989</v>
+        <v>667.8988417941412</v>
       </c>
     </row>
     <row r="299">
       <c r="A299" t="n">
-        <v>708.140682261984</v>
+        <v>674.1271107944726</v>
       </c>
     </row>
     <row r="300">
       <c r="A300" t="n">
-        <v>710.5463435210879</v>
+        <v>694.746466178799</v>
       </c>
     </row>
     <row r="301">
       <c r="A301" t="n">
-        <v>727.7362964351823</v>
+        <v>699.2626634826422</v>
       </c>
     </row>
     <row r="302">
       <c r="A302" t="n">
-        <v>683.3996249472136</v>
+        <v>719.0855420624018</v>
       </c>
     </row>
     <row r="303">
       <c r="A303" t="n">
-        <v>581.1437510170094</v>
+        <v>686.0775150671827</v>
       </c>
     </row>
     <row r="304">
       <c r="A304" t="n">
-        <v>537.7332390075935</v>
+        <v>587.9019052258911</v>
       </c>
     </row>
     <row r="305">
       <c r="A305" t="n">
-        <v>545.3505403141321</v>
+        <v>536.4854351957717</v>
       </c>
     </row>
     <row r="306">
       <c r="A306" t="n">
-        <v>558.7397112851136</v>
+        <v>537.9418614543852</v>
       </c>
     </row>
     <row r="307">
       <c r="A307" t="n">
-        <v>556.2247141775458</v>
+        <v>551.1356130477338</v>
       </c>
     </row>
     <row r="308">
       <c r="A308" t="n">
-        <v>532.8222607538748</v>
+        <v>551.4517752696406</v>
       </c>
     </row>
     <row r="309">
       <c r="A309" t="n">
-        <v>510.5648256912332</v>
+        <v>530.9645252306154</v>
       </c>
     </row>
     <row r="310">
       <c r="A310" t="n">
-        <v>494.604684007669</v>
+        <v>509.43386376386</v>
       </c>
     </row>
     <row r="311">
       <c r="A311" t="n">
-        <v>500.5985477004629</v>
+        <v>490.8194858796833</v>
       </c>
     </row>
     <row r="312">
       <c r="A312" t="n">
-        <v>491.5232245544701</v>
+        <v>492.7371934926441</v>
       </c>
     </row>
     <row r="313">
       <c r="A313" t="n">
-        <v>520.90504483877</v>
+        <v>487.334978262993</v>
       </c>
     </row>
     <row r="314">
       <c r="A314" t="n">
-        <v>553.3248176901679</v>
+        <v>517.7357200451809</v>
       </c>
     </row>
     <row r="315">
       <c r="A315" t="n">
-        <v>560.9348365533151</v>
+        <v>551.9969367854571</v>
       </c>
     </row>
     <row r="316">
       <c r="A316" t="n">
-        <v>589.7439766756065</v>
+        <v>557.8363324900124</v>
       </c>
     </row>
     <row r="317">
       <c r="A317" t="n">
-        <v>666.68132830236</v>
+        <v>575.1892001758847</v>
       </c>
     </row>
     <row r="318">
       <c r="A318" t="n">
-        <v>700.7774178158286</v>
+        <v>644.5835890785077</v>
       </c>
     </row>
     <row r="319">
       <c r="A319" t="n">
-        <v>719.5183964953458</v>
+        <v>679.2064373908886</v>
       </c>
     </row>
     <row r="320">
       <c r="A320" t="n">
-        <v>661.7812204356142</v>
+        <v>708.4125078713157</v>
       </c>
     </row>
     <row r="321">
       <c r="A321" t="n">
-        <v>615.4589839240998</v>
+        <v>662.3661847812343</v>
       </c>
     </row>
     <row r="322">
       <c r="A322" t="n">
-        <v>617.2388320011919</v>
+        <v>611.2658735852676</v>
       </c>
     </row>
     <row r="323">
       <c r="A323" t="n">
-        <v>643.0971768855045</v>
+        <v>619.9642736781357</v>
       </c>
     </row>
     <row r="324">
       <c r="A324" t="n">
-        <v>714.2419535701663</v>
+        <v>640.9113954061922</v>
       </c>
     </row>
     <row r="325">
       <c r="A325" t="n">
-        <v>715.1629109780799</v>
+        <v>709.2999355748475</v>
       </c>
     </row>
     <row r="326">
       <c r="A326" t="n">
-        <v>705.7532019236703</v>
+        <v>720.6810961869792</v>
       </c>
     </row>
     <row r="327">
       <c r="A327" t="n">
-        <v>682.4813236725049</v>
+        <v>704.7888314505713</v>
       </c>
     </row>
     <row r="328">
       <c r="A328" t="n">
-        <v>631.6493271676222</v>
+        <v>678.2185811826196</v>
       </c>
     </row>
     <row r="329">
       <c r="A329" t="n">
-        <v>627.1656652565696</v>
+        <v>634.1629173513752</v>
       </c>
     </row>
     <row r="330">
       <c r="A330" t="n">
-        <v>631.4555549268448</v>
+        <v>617.878918859617</v>
       </c>
     </row>
     <row r="331">
       <c r="A331" t="n">
-        <v>662.2351937465965</v>
+        <v>626.6161959108274</v>
       </c>
     </row>
     <row r="332">
       <c r="A332" t="n">
-        <v>738.9035428435307</v>
+        <v>645.8690842884494</v>
       </c>
     </row>
     <row r="333">
       <c r="A333" t="n">
-        <v>771.2233637761301</v>
+        <v>722.8070732323602</v>
       </c>
     </row>
     <row r="334">
       <c r="A334" t="n">
-        <v>707.1172889380932</v>
+        <v>772.9607378629169</v>
       </c>
     </row>
     <row r="335">
       <c r="A335" t="n">
-        <v>687.380893970186</v>
+        <v>717.3066342360244</v>
       </c>
     </row>
     <row r="336">
       <c r="A336" t="n">
-        <v>722.2811009331735</v>
+        <v>675.9046814154317</v>
       </c>
     </row>
     <row r="337">
       <c r="A337" t="n">
-        <v>780.9991421561335</v>
+        <v>708.7328218649418</v>
       </c>
     </row>
     <row r="338">
       <c r="A338" t="n">
-        <v>771.8500920253177</v>
+        <v>762.9697838474101</v>
       </c>
     </row>
     <row r="339">
       <c r="A339" t="n">
-        <v>690.6818756503128</v>
+        <v>782.8416902961521</v>
       </c>
     </row>
     <row r="340">
       <c r="A340" t="n">
-        <v>633.6147790144935</v>
+        <v>713.7793197170197</v>
       </c>
     </row>
     <row r="341">
       <c r="A341" t="n">
-        <v>646.2809956928197</v>
+        <v>637.7621539429299</v>
       </c>
     </row>
     <row r="342">
       <c r="A342" t="n">
-        <v>655.1157509130974</v>
+        <v>633.0638650355809</v>
       </c>
     </row>
     <row r="343">
       <c r="A343" t="n">
-        <v>604.3274758729069</v>
+        <v>659.8003387395579</v>
       </c>
     </row>
     <row r="344">
       <c r="A344" t="n">
-        <v>614.1516569274756</v>
+        <v>615.7851344848098</v>
       </c>
     </row>
     <row r="345">
       <c r="A345" t="n">
-        <v>688.6532134082017</v>
+        <v>600.9546894465529</v>
       </c>
     </row>
     <row r="346">
       <c r="A346" t="n">
-        <v>723.4147560326676</v>
+        <v>670.0620222271425</v>
       </c>
     </row>
     <row r="347">
       <c r="A347" t="n">
-        <v>675.9337013463949</v>
+        <v>718.6069440975871</v>
       </c>
     </row>
     <row r="348">
       <c r="A348" t="n">
-        <v>669.0494307033532</v>
+        <v>689.6908016536827</v>
       </c>
     </row>
     <row r="349">
       <c r="A349" t="n">
-        <v>623.6124881120304</v>
+        <v>665.6404064419803</v>
       </c>
     </row>
     <row r="350">
       <c r="A350" t="n">
-        <v>552.6140844338556</v>
+        <v>641.7837035630782</v>
       </c>
     </row>
     <row r="351">
       <c r="A351" t="n">
-        <v>525.5085400671078</v>
+        <v>564.0713445504844</v>
       </c>
     </row>
     <row r="352">
       <c r="A352" t="n">
-        <v>504.2930655969826</v>
+        <v>530.8844062956837</v>
       </c>
     </row>
     <row r="353">
       <c r="A353" t="n">
-        <v>536.1978526779296</v>
+        <v>502.6836795092038</v>
       </c>
     </row>
     <row r="354">
       <c r="A354" t="n">
-        <v>607.2009538179088</v>
+        <v>517.0282678191711</v>
       </c>
     </row>
     <row r="355">
       <c r="A355" t="n">
-        <v>676.2356399674445</v>
+        <v>586.7586398330218</v>
       </c>
     </row>
     <row r="356">
       <c r="A356" t="n">
-        <v>731.0630910732243</v>
+        <v>659.4717459791752</v>
       </c>
     </row>
     <row r="357">
       <c r="A357" t="n">
-        <v>740.5510715339005</v>
+        <v>725.0538040300967</v>
       </c>
     </row>
     <row r="358">
       <c r="A358" t="n">
-        <v>740.6080565938851</v>
+        <v>742.611215105768</v>
       </c>
     </row>
     <row r="359">
       <c r="A359" t="n">
-        <v>743.9367261191592</v>
+        <v>743.1951787891933</v>
       </c>
     </row>
     <row r="360">
       <c r="A360" t="n">
-        <v>751.2405048066739</v>
+        <v>741.2947141521613</v>
       </c>
     </row>
     <row r="361">
       <c r="A361" t="n">
-        <v>680.2671258411692</v>
+        <v>762.3908675291204</v>
       </c>
     </row>
     <row r="362">
       <c r="A362" t="n">
-        <v>610.1473740642973</v>
+        <v>699.2030938356777</v>
       </c>
     </row>
     <row r="363">
       <c r="A363" t="n">
-        <v>580.2508055005262</v>
+        <v>623.571230607439</v>
       </c>
     </row>
     <row r="364">
       <c r="A364" t="n">
-        <v>574.4831228089424</v>
+        <v>591.4237992608662</v>
       </c>
     </row>
     <row r="365">
       <c r="A365" t="n">
-        <v>599.0318785323723</v>
+        <v>566.5086740196443</v>
       </c>
     </row>
     <row r="366">
       <c r="A366" t="n">
-        <v>615.1633954642648</v>
+        <v>591.2952480162517</v>
       </c>
     </row>
     <row r="367">
       <c r="A367" t="n">
-        <v>616.3017593380857</v>
+        <v>613.7139534346829</v>
       </c>
     </row>
     <row r="368">
       <c r="A368" t="n">
-        <v>631.5062553395876</v>
+        <v>610.0311086487409</v>
       </c>
     </row>
     <row r="369">
       <c r="A369" t="n">
-        <v>668.9374673344162</v>
+        <v>623.6231353663584</v>
       </c>
     </row>
     <row r="370">
       <c r="A370" t="n">
-        <v>756.0587660473743</v>
+        <v>649.6831674476198</v>
       </c>
     </row>
     <row r="371">
       <c r="A371" t="n">
-        <v>776.5695371922732</v>
+        <v>735.0652459227831</v>
       </c>
     </row>
     <row r="372">
       <c r="A372" t="n">
-        <v>677.0750706328954</v>
+        <v>787.6239617068279</v>
       </c>
     </row>
     <row r="373">
       <c r="A373" t="n">
-        <v>626.2003424591853</v>
+        <v>705.8795087762633</v>
       </c>
     </row>
     <row r="374">
       <c r="A374" t="n">
-        <v>625.3684638870993</v>
+        <v>623.6333213934699</v>
       </c>
     </row>
     <row r="375">
       <c r="A375" t="n">
-        <v>626.4904746665252</v>
+        <v>616.4409530416322</v>
       </c>
     </row>
     <row r="376">
       <c r="A376" t="n">
-        <v>627.1436137795945</v>
+        <v>628.2318698767995</v>
       </c>
     </row>
     <row r="377">
       <c r="A377" t="n">
-        <v>672.9333652248215</v>
+        <v>615.5791059253204</v>
       </c>
     </row>
     <row r="378">
       <c r="A378" t="n">
-        <v>669.2720032550881</v>
+        <v>649.4935131596549</v>
       </c>
     </row>
     <row r="379">
       <c r="A379" t="n">
-        <v>650.0481061749497</v>
+        <v>674.4471270651218</v>
       </c>
     </row>
     <row r="380">
       <c r="A380" t="n">
-        <v>663.4908089203009</v>
+        <v>647.7846678053538</v>
       </c>
     </row>
     <row r="381">
       <c r="A381" t="n">
-        <v>682.2032443713226</v>
+        <v>652.9814187163652</v>
       </c>
     </row>
     <row r="382">
       <c r="A382" t="n">
-        <v>636.68840383869</v>
+        <v>681.8067400980112</v>
       </c>
     </row>
     <row r="383">
       <c r="A383" t="n">
-        <v>570.93331897903</v>
+        <v>657.6919526489462</v>
       </c>
     </row>
     <row r="384">
       <c r="A384" t="n">
-        <v>537.8585045670548</v>
+        <v>589.8360046144546</v>
       </c>
     </row>
     <row r="385">
       <c r="A385" t="n">
-        <v>573.2117521945668</v>
+        <v>546.8429916367086</v>
       </c>
     </row>
     <row r="386">
       <c r="A386" t="n">
-        <v>610.3418542999748</v>
+        <v>554.4714941750613</v>
       </c>
     </row>
     <row r="387">
       <c r="A387" t="n">
-        <v>649.2103694432387</v>
+        <v>594.0204679475585</v>
       </c>
     </row>
     <row r="388">
       <c r="A388" t="n">
-        <v>671.9180229210053</v>
+        <v>643.7548797247814</v>
       </c>
     </row>
     <row r="389">
       <c r="A389" t="n">
-        <v>719.2656405397031</v>
+        <v>642.9857634292375</v>
       </c>
     </row>
     <row r="390">
       <c r="A390" t="n">
-        <v>674.3995044342057</v>
+        <v>711.9849923714128</v>
       </c>
     </row>
     <row r="391">
       <c r="A391" t="n">
-        <v>700.4475452264387</v>
+        <v>692.1728123100479</v>
       </c>
     </row>
     <row r="392">
       <c r="A392" t="n">
-        <v>682.1669979519243</v>
+        <v>686.2351785876797</v>
       </c>
     </row>
     <row r="393">
       <c r="A393" t="n">
-        <v>706.3857431591316</v>
+        <v>695.9495934041229</v>
       </c>
     </row>
     <row r="394">
       <c r="A394" t="n">
-        <v>692.5375373313329</v>
+        <v>709.5864414068842</v>
       </c>
     </row>
     <row r="395">
       <c r="A395" t="n">
-        <v>634.3698136642217</v>
+        <v>695.9096982085384</v>
       </c>
     </row>
     <row r="396">
       <c r="A396" t="n">
-        <v>557.0261197406978</v>
+        <v>666.0515223425421</v>
       </c>
     </row>
     <row r="397">
       <c r="A397" t="n">
-        <v>522.8504674679186</v>
+        <v>581.6310680596359</v>
       </c>
     </row>
     <row r="398">
       <c r="A398" t="n">
-        <v>516.23689492925</v>
+        <v>536.379060575257</v>
       </c>
     </row>
     <row r="399">
       <c r="A399" t="n">
-        <v>540.1988350339764</v>
+        <v>520.1126907190314</v>
       </c>
     </row>
     <row r="400">
       <c r="A400" t="n">
-        <v>560.9173079125753</v>
+        <v>524.2808607928566</v>
       </c>
     </row>
     <row r="401">
       <c r="A401" t="n">
-        <v>577.0907541765098</v>
+        <v>555.1366888922473</v>
       </c>
     </row>
     <row r="402">
       <c r="A402" t="n">
-        <v>593.6118433854176</v>
+        <v>577.8395021644656</v>
       </c>
     </row>
     <row r="403">
       <c r="A403" t="n">
-        <v>629.8638856970626</v>
+        <v>595.7116476282351</v>
       </c>
     </row>
     <row r="404">
       <c r="A404" t="n">
-        <v>666.7499417472698</v>
+        <v>611.7487563017505</v>
       </c>
     </row>
     <row r="405">
       <c r="A405" t="n">
-        <v>663.8185701200712</v>
+        <v>653.0412636443543</v>
       </c>
     </row>
     <row r="406">
       <c r="A406" t="n">
-        <v>664.169872565509</v>
+        <v>663.3781829261238</v>
       </c>
     </row>
     <row r="407">
       <c r="A407" t="n">
-        <v>616.230240487539</v>
+        <v>660.9096788507713</v>
       </c>
     </row>
     <row r="408">
       <c r="A408" t="n">
-        <v>577.7195824813646</v>
+        <v>633.9582611787762</v>
       </c>
     </row>
     <row r="409">
       <c r="A409" t="n">
-        <v>515.5805615152929</v>
+        <v>596.4691011099603</v>
       </c>
     </row>
     <row r="410">
       <c r="A410" t="n">
-        <v>451.1533294410413</v>
+        <v>545.2851292326955</v>
       </c>
     </row>
     <row r="411">
       <c r="A411" t="n">
-        <v>450.3524871984155</v>
+        <v>475.978754763247</v>
       </c>
     </row>
     <row r="412">
       <c r="A412" t="n">
-        <v>459.310770134266</v>
+        <v>443.5860443921911</v>
       </c>
     </row>
     <row r="413">
       <c r="A413" t="n">
-        <v>485.6590206292708</v>
+        <v>453.8568811159109</v>
       </c>
     </row>
     <row r="414">
       <c r="A414" t="n">
-        <v>506.4551994457815</v>
+        <v>469.3983066469798</v>
       </c>
     </row>
     <row r="415">
       <c r="A415" t="n">
-        <v>528.7050495248877</v>
+        <v>490.2437063258844</v>
       </c>
     </row>
     <row r="416">
       <c r="A416" t="n">
-        <v>621.0093753995807</v>
+        <v>506.3203673369117</v>
       </c>
     </row>
     <row r="417">
       <c r="A417" t="n">
-        <v>732.9305952591767</v>
+        <v>558.8795396395767</v>
       </c>
     </row>
     <row r="418">
       <c r="A418" t="n">
-        <v>802.5086317560977</v>
+        <v>680.4448952231041</v>
       </c>
     </row>
     <row r="419">
       <c r="A419" t="n">
-        <v>805.6524571653654</v>
+        <v>777.611508097948</v>
       </c>
     </row>
     <row r="420">
       <c r="A420" t="n">
-        <v>736.0275426514704</v>
+        <v>819.9082549422201</v>
       </c>
     </row>
     <row r="421">
       <c r="A421" t="n">
-        <v>685.6847629405252</v>
+        <v>796.8598940506126</v>
       </c>
     </row>
     <row r="422">
       <c r="A422" t="n">
-        <v>688.0665759345561</v>
+        <v>723.1720428499102</v>
       </c>
     </row>
     <row r="423">
       <c r="A423" t="n">
-        <v>713.5680897488896</v>
+        <v>686.8887005944089</v>
       </c>
     </row>
     <row r="424">
       <c r="A424" t="n">
-        <v>735.7844791280854</v>
+        <v>694.619982156496</v>
       </c>
     </row>
     <row r="425">
       <c r="A425" t="n">
-        <v>750.2528788857035</v>
+        <v>743.943001286425</v>
       </c>
     </row>
     <row r="426">
       <c r="A426" t="n">
-        <v>743.2446715849323</v>
+        <v>730.7035998991864</v>
       </c>
     </row>
     <row r="427">
       <c r="A427" t="n">
-        <v>759.0023934110377</v>
+        <v>722.7136791140651</v>
       </c>
     </row>
     <row r="428">
       <c r="A428" t="n">
-        <v>746.6523690462168</v>
+        <v>731.879489345431</v>
       </c>
     </row>
     <row r="429">
       <c r="A429" t="n">
-        <v>685.766302524712</v>
+        <v>747.6521133090159</v>
       </c>
     </row>
     <row r="430">
       <c r="A430" t="n">
-        <v>663.9833896109053</v>
+        <v>715.6450741160256</v>
       </c>
     </row>
     <row r="431">
       <c r="A431" t="n">
-        <v>698.8711756480939</v>
+        <v>666.882001397596</v>
       </c>
     </row>
     <row r="432">
       <c r="A432" t="n">
-        <v>679.6542390105742</v>
+        <v>712.3320762188428</v>
       </c>
     </row>
     <row r="433">
       <c r="A433" t="n">
-        <v>692.6960022268531</v>
+        <v>690.4080982284313</v>
       </c>
     </row>
     <row r="434">
       <c r="A434" t="n">
-        <v>698.7527291005904</v>
+        <v>683.480734981913</v>
       </c>
     </row>
     <row r="435">
       <c r="A435" t="n">
-        <v>664.6737896300579</v>
+        <v>712.3722830313568</v>
       </c>
     </row>
     <row r="436">
       <c r="A436" t="n">
-        <v>628.6527236520669</v>
+        <v>696.8086902090249</v>
       </c>
     </row>
     <row r="437">
       <c r="A437" t="n">
-        <v>643.736815076636</v>
+        <v>646.8054979409317</v>
       </c>
     </row>
     <row r="438">
       <c r="A438" t="n">
-        <v>724.2793971483934</v>
+        <v>648.0882549006992</v>
       </c>
     </row>
     <row r="439">
       <c r="A439" t="n">
-        <v>726.8912936912102</v>
+        <v>708.749496970313</v>
       </c>
     </row>
     <row r="440">
       <c r="A440" t="n">
-        <v>708.2582843610794</v>
+        <v>754.1963694676497</v>
       </c>
     </row>
     <row r="441">
       <c r="A441" t="n">
-        <v>673.8854901780087</v>
+        <v>718.9164999632567</v>
       </c>
     </row>
     <row r="442">
       <c r="A442" t="n">
-        <v>650.3338188533121</v>
+        <v>694.6690475974151</v>
       </c>
     </row>
     <row r="443">
       <c r="A443" t="n">
-        <v>639.5827118581678</v>
+        <v>657.7911375149483</v>
       </c>
     </row>
     <row r="444">
       <c r="A444" t="n">
-        <v>621.6764370774399</v>
+        <v>632.0467174990085</v>
       </c>
     </row>
     <row r="445">
       <c r="A445" t="n">
-        <v>627.5970298610218</v>
+        <v>619.2153202352415</v>
       </c>
     </row>
     <row r="446">
       <c r="A446" t="n">
-        <v>655.8936596865124</v>
+        <v>622.5888611043047</v>
       </c>
     </row>
     <row r="447">
       <c r="A447" t="n">
-        <v>668.2385866043887</v>
+        <v>634.8956922390698</v>
       </c>
     </row>
     <row r="448">
       <c r="A448" t="n">
-        <v>710.8986470419154</v>
+        <v>653.698336394541</v>
       </c>
     </row>
     <row r="449">
       <c r="A449" t="n">
-        <v>769.2336728289888</v>
+        <v>674.7224949309611</v>
       </c>
     </row>
     <row r="450">
       <c r="A450" t="n">
-        <v>747.1092190747868</v>
+        <v>736.3716388187527</v>
       </c>
     </row>
     <row r="451">
       <c r="A451" t="n">
-        <v>665.9024146408115</v>
+        <v>766.1645651007802</v>
       </c>
     </row>
     <row r="452">
       <c r="A452" t="n">
-        <v>594.1250254297188</v>
+        <v>708.7251267767556</v>
       </c>
     </row>
     <row r="453">
       <c r="A453" t="n">
-        <v>588.6053399316893</v>
+        <v>626.6823367542997</v>
       </c>
     </row>
     <row r="454">
       <c r="A454" t="n">
-        <v>589.8669398640664</v>
+        <v>599.8702015550634</v>
       </c>
     </row>
     <row r="455">
       <c r="A455" t="n">
-        <v>612.9153306690114</v>
+        <v>584.4313740755069</v>
       </c>
     </row>
     <row r="456">
       <c r="A456" t="n">
-        <v>593.4044958305549</v>
+        <v>612.6144927135329</v>
       </c>
     </row>
     <row r="457">
       <c r="A457" t="n">
-        <v>613.6468404812376</v>
+        <v>584.4674923810658</v>
       </c>
     </row>
     <row r="458">
       <c r="A458" t="n">
-        <v>623.2493947925946</v>
+        <v>594.8445039889521</v>
       </c>
     </row>
     <row r="459">
       <c r="A459" t="n">
-        <v>657.0606949343301</v>
+        <v>604.4873298221205</v>
       </c>
     </row>
     <row r="460">
       <c r="A460" t="n">
-        <v>686.919243421471</v>
+        <v>636.453417220423</v>
       </c>
     </row>
     <row r="461">
       <c r="A461" t="n">
-        <v>691.7935780484186</v>
+        <v>643.6520613419248</v>
       </c>
     </row>
     <row r="462">
       <c r="A462" t="n">
-        <v>641.1702345729395</v>
+        <v>676.0799163653246</v>
       </c>
     </row>
     <row r="463">
       <c r="A463" t="n">
-        <v>583.8630159939839</v>
+        <v>664.6501647858827</v>
       </c>
     </row>
     <row r="464">
       <c r="A464" t="n">
-        <v>606.34798056725</v>
+        <v>621.8361246712334</v>
       </c>
     </row>
     <row r="465">
       <c r="A465" t="n">
-        <v>610.6675722410841</v>
+        <v>635.23662188868</v>
       </c>
     </row>
     <row r="466">
       <c r="A466" t="n">
-        <v>578.2678313003657</v>
+        <v>647.7072887372515</v>
       </c>
     </row>
     <row r="467">
       <c r="A467" t="n">
-        <v>599.7278132037422</v>
+        <v>616.0150395072037</v>
       </c>
     </row>
     <row r="468">
       <c r="A468" t="n">
-        <v>598.9179735993844</v>
+        <v>614.9796076339271</v>
       </c>
     </row>
     <row r="469">
       <c r="A469" t="n">
-        <v>676.0767994505841</v>
+        <v>614.3684524215018</v>
       </c>
     </row>
     <row r="470">
       <c r="A470" t="n">
-        <v>719.9279957394538</v>
+        <v>662.9036581285277</v>
       </c>
     </row>
     <row r="471">
       <c r="A471" t="n">
-        <v>677.2266786976502</v>
+        <v>699.6139654687568</v>
       </c>
     </row>
     <row r="472">
       <c r="A472" t="n">
-        <v>623.7710135656584</v>
+        <v>660.6253479262136</v>
       </c>
     </row>
     <row r="473">
       <c r="A473" t="n">
-        <v>616.9190264331519</v>
+        <v>587.5425836999852</v>
       </c>
     </row>
     <row r="474">
       <c r="A474" t="n">
-        <v>612.1524731760246</v>
+        <v>588.10890175846</v>
       </c>
     </row>
     <row r="475">
       <c r="A475" t="n">
-        <v>656.1881933010909</v>
+        <v>599.3161796528739</v>
       </c>
     </row>
     <row r="476">
       <c r="A476" t="n">
-        <v>616.1458913484807</v>
+        <v>654.6381679435171</v>
       </c>
     </row>
     <row r="477">
       <c r="A477" t="n">
-        <v>505.0205516646429</v>
+        <v>651.0987761193974</v>
       </c>
     </row>
     <row r="478">
       <c r="A478" t="n">
-        <v>516.3757721365414</v>
+        <v>555.7864120586373</v>
       </c>
     </row>
     <row r="479">
       <c r="A479" t="n">
-        <v>551.6691517690901</v>
+        <v>540.395436099061</v>
       </c>
     </row>
     <row r="480">
       <c r="A480" t="n">
-        <v>565.0237422059945</v>
+        <v>565.1443685101754</v>
       </c>
     </row>
     <row r="481">
       <c r="A481" t="n">
-        <v>593.9707867821085</v>
+        <v>577.0220982406045</v>
       </c>
     </row>
     <row r="482">
       <c r="A482" t="n">
-        <v>648.4811414225646</v>
+        <v>585.5042092670715</v>
       </c>
     </row>
     <row r="483">
       <c r="A483" t="n">
-        <v>632.8677896482873</v>
+        <v>651.6100191346368</v>
       </c>
     </row>
     <row r="484">
       <c r="A484" t="n">
-        <v>632.879039037789</v>
+        <v>652.0472956299841</v>
       </c>
     </row>
     <row r="485">
       <c r="A485" t="n">
-        <v>671.0026279473027</v>
+        <v>627.6267818239489</v>
       </c>
     </row>
     <row r="486">
       <c r="A486" t="n">
-        <v>698.587060399916</v>
+        <v>639.8601284048482</v>
       </c>
     </row>
     <row r="487">
       <c r="A487" t="n">
-        <v>639.400746816932</v>
+        <v>669.5587249325285</v>
       </c>
     </row>
     <row r="488">
       <c r="A488" t="n">
-        <v>624.3420289118831</v>
+        <v>643.622389115535</v>
       </c>
     </row>
     <row r="489">
       <c r="A489" t="n">
-        <v>650.9503311348794</v>
+        <v>637.7173596314947</v>
       </c>
     </row>
     <row r="490">
       <c r="A490" t="n">
-        <v>651.5776525671413</v>
+        <v>678.5470742673283</v>
       </c>
     </row>
     <row r="491">
       <c r="A491" t="n">
-        <v>600.9096812366579</v>
+        <v>678.2682017073398</v>
       </c>
     </row>
     <row r="492">
       <c r="A492" t="n">
-        <v>556.5211631184752</v>
+        <v>632.1235716212641</v>
       </c>
     </row>
     <row r="493">
       <c r="A493" t="n">
-        <v>582.6871538889122</v>
+        <v>569.6236395975234</v>
       </c>
     </row>
     <row r="494">
       <c r="A494" t="n">
-        <v>604.7394080033541</v>
+        <v>580.5431944984889</v>
       </c>
     </row>
     <row r="495">
       <c r="A495" t="n">
-        <v>616.4317697976571</v>
+        <v>589.5742633342138</v>
       </c>
     </row>
     <row r="496">
       <c r="A496" t="n">
-        <v>681.6641481452166</v>
+        <v>587.2251338888645</v>
       </c>
     </row>
     <row r="497">
       <c r="A497" t="n">
-        <v>748.9455486437464</v>
+        <v>644.8634580473254</v>
       </c>
     </row>
     <row r="498">
       <c r="A498" t="n">
-        <v>784.2464425445428</v>
+        <v>760.9509213677939</v>
       </c>
     </row>
     <row r="499">
       <c r="A499" t="n">
-        <v>854.9250296210289</v>
+        <v>791.399877505512</v>
       </c>
     </row>
     <row r="500">
       <c r="A500" t="n">
-        <v>871.1496980721449</v>
+        <v>864.7500213131138</v>
       </c>
     </row>
     <row r="501">
       <c r="A501" t="n">
-        <v>752.9337073347051</v>
+        <v>892.0332181004937</v>
       </c>
     </row>
     <row r="502">
       <c r="A502" t="n">
-        <v>748.3287619832595</v>
+        <v>765.6201431628915</v>
       </c>
     </row>
     <row r="503">
       <c r="A503" t="n">
-        <v>781.1265197368016</v>
+        <v>766.8370242474225</v>
       </c>
     </row>
     <row r="504">
       <c r="A504" t="n">
-        <v>749.7426247252861</v>
+        <v>795.2829165121216</v>
       </c>
     </row>
     <row r="505">
       <c r="A505" t="n">
-        <v>747.2178418035469</v>
+        <v>753.2357398729346</v>
       </c>
     </row>
     <row r="506">
       <c r="A506" t="n">
-        <v>670.4361573335973</v>
+        <v>756.4704690919939</v>
       </c>
     </row>
     <row r="507">
       <c r="A507" t="n">
-        <v>599.8905443660192</v>
+        <v>687.7059284872757</v>
       </c>
     </row>
     <row r="508">
       <c r="A508" t="n">
-        <v>637.8493600581692</v>
+        <v>628.0939582160272</v>
       </c>
     </row>
     <row r="509">
       <c r="A509" t="n">
-        <v>674.2168327835998</v>
+        <v>677.4580542268609</v>
       </c>
     </row>
     <row r="510">
       <c r="A510" t="n">
-        <v>608.4941347170911</v>
+        <v>693.4381273674148</v>
       </c>
     </row>
     <row r="511">
       <c r="A511" t="n">
-        <v>630.5190917575487</v>
+        <v>614.7719148343072</v>
       </c>
     </row>
     <row r="512">
       <c r="A512" t="n">
-        <v>679.6479367522466</v>
+        <v>656.1052911079628</v>
       </c>
     </row>
     <row r="513">
       <c r="A513" t="n">
-        <v>652.2587453020492</v>
+        <v>678.0691192859081</v>
       </c>
     </row>
     <row r="514">
       <c r="A514" t="n">
-        <v>702.2776475553769</v>
+        <v>666.9118026407546</v>
       </c>
     </row>
     <row r="515">
       <c r="A515" t="n">
-        <v>709.531768066995</v>
+        <v>731.8130428729432</v>
       </c>
     </row>
     <row r="516">
       <c r="A516" t="n">
-        <v>666.7630631317252</v>
+        <v>719.4736796687948</v>
       </c>
     </row>
     <row r="517">
       <c r="A517" t="n">
-        <v>698.4358640011692</v>
+        <v>674.4528409099644</v>
       </c>
     </row>
     <row r="518">
       <c r="A518" t="n">
-        <v>766.5485170668944</v>
+        <v>722.0423395023658</v>
       </c>
     </row>
     <row r="519">
       <c r="A519" t="n">
-        <v>790.1701669941872</v>
+        <v>767.975334763662</v>
       </c>
     </row>
     <row r="520">
       <c r="A520" t="n">
-        <v>720.9831027417408</v>
+        <v>758.396455386503</v>
       </c>
     </row>
     <row r="521">
       <c r="A521" t="n">
-        <v>724.377406383212</v>
+        <v>708.1212422970111</v>
       </c>
     </row>
     <row r="522">
       <c r="A522" t="n">
-        <v>788.2238440423066</v>
+        <v>758.5742993478561</v>
       </c>
     </row>
     <row r="523">
       <c r="A523" t="n">
-        <v>711.390939399962</v>
+        <v>792.4557940042973</v>
       </c>
     </row>
     <row r="524">
       <c r="A524" t="n">
-        <v>671.9374309516866</v>
+        <v>684.8765792108793</v>
       </c>
     </row>
     <row r="525">
       <c r="A525" t="n">
-        <v>666.2002292476927</v>
+        <v>684.324018671532</v>
       </c>
     </row>
     <row r="526">
       <c r="A526" t="n">
-        <v>677.5855139880491</v>
+        <v>681.2239572264502</v>
       </c>
     </row>
     <row r="527">
       <c r="A527" t="n">
-        <v>688.890169293245</v>
+        <v>675.9214373947202</v>
       </c>
     </row>
     <row r="528">
       <c r="A528" t="n">
-        <v>709.3235131086999</v>
+        <v>696.015224840437</v>
       </c>
     </row>
     <row r="529">
       <c r="A529" t="n">
-        <v>705.3896878949217</v>
+        <v>706.2703633908427</v>
       </c>
     </row>
     <row r="530">
       <c r="A530" t="n">
-        <v>735.3436024432085</v>
+        <v>707.1554766168902</v>
       </c>
     </row>
     <row r="531">
       <c r="A531" t="n">
-        <v>741.4848420180533</v>
+        <v>747.7386275377285</v>
       </c>
     </row>
     <row r="532">
       <c r="A532" t="n">
-        <v>706.2258274985425</v>
+        <v>761.088769511332</v>
       </c>
     </row>
     <row r="533">
       <c r="A533" t="n">
-        <v>611.8412409676353</v>
+        <v>666.4748089296495</v>
       </c>
     </row>
     <row r="534">
       <c r="A534" t="n">
-        <v>589.3598522112029</v>
+        <v>589.6313272816087</v>
       </c>
     </row>
     <row r="535">
       <c r="A535" t="n">
-        <v>601.5071412161888</v>
+        <v>580.7574540344262</v>
       </c>
     </row>
     <row r="536">
       <c r="A536" t="n">
-        <v>615.8358085671694</v>
+        <v>593.5294927562609</v>
       </c>
     </row>
     <row r="537">
       <c r="A537" t="n">
-        <v>633.8705811830891</v>
+        <v>613.0317199534261</v>
       </c>
     </row>
     <row r="538">
       <c r="A538" t="n">
-        <v>700.8687209128084</v>
+        <v>646.7328214544636</v>
       </c>
     </row>
     <row r="539">
       <c r="A539" t="n">
-        <v>725.0401773787303</v>
+        <v>722.0509613152899</v>
       </c>
     </row>
     <row r="540">
       <c r="A540" t="n">
-        <v>697.3943596213417</v>
+        <v>720.9775836208792</v>
       </c>
     </row>
     <row r="541">
       <c r="A541" t="n">
-        <v>765.3040691879482</v>
+        <v>717.5516180857358</v>
       </c>
     </row>
     <row r="542">
       <c r="A542" t="n">
-        <v>743.8354866746977</v>
+        <v>780.6014551977114</v>
       </c>
     </row>
     <row r="543">
       <c r="A543" t="n">
-        <v>697.1147977322971</v>
+        <v>735.9297301624679</v>
       </c>
     </row>
     <row r="544">
       <c r="A544" t="n">
-        <v>709.746809692831</v>
+        <v>709.6732961645102</v>
       </c>
     </row>
     <row r="545">
       <c r="A545" t="n">
-        <v>680.5773406871367</v>
+        <v>717.4639814082298</v>
       </c>
     </row>
     <row r="546">
       <c r="A546" t="n">
-        <v>621.9278870112817</v>
+        <v>668.7346454993985</v>
       </c>
     </row>
     <row r="547">
       <c r="A547" t="n">
-        <v>579.922960404474</v>
+        <v>607.7537088263512</v>
       </c>
     </row>
     <row r="548">
       <c r="A548" t="n">
-        <v>500.3261537423782</v>
+        <v>535.8909543771802</v>
       </c>
     </row>
     <row r="549">
       <c r="A549" t="n">
-        <v>485.3307312397419</v>
+        <v>485.3639728689814</v>
       </c>
     </row>
     <row r="550">
       <c r="A550" t="n">
-        <v>490.5380747718482</v>
+        <v>489.9800152579701</v>
       </c>
     </row>
     <row r="551">
       <c r="A551" t="n">
-        <v>511.295748429518</v>
+        <v>493.3808283248595</v>
       </c>
     </row>
     <row r="552">
       <c r="A552" t="n">
-        <v>610.3521359192428</v>
+        <v>532.3097380510831</v>
       </c>
     </row>
     <row r="553">
       <c r="A553" t="n">
-        <v>668.0423634362</v>
+        <v>628.1747562745181</v>
       </c>
     </row>
     <row r="554">
       <c r="A554" t="n">
-        <v>685.013383523426</v>
+        <v>678.6782535376119</v>
       </c>
     </row>
     <row r="555">
       <c r="A555" t="n">
-        <v>733.4719090679869</v>
+        <v>714.7596356390977</v>
       </c>
     </row>
     <row r="556">
       <c r="A556" t="n">
-        <v>720.6816244838024</v>
+        <v>748.6152492417659</v>
       </c>
     </row>
     <row r="557">
       <c r="A557" t="n">
-        <v>707.23719112749</v>
+        <v>722.1906844087016</v>
       </c>
     </row>
     <row r="558">
       <c r="A558" t="n">
-        <v>639.6160738730146</v>
+        <v>696.8676959501749</v>
       </c>
     </row>
     <row r="559">
       <c r="A559" t="n">
-        <v>620.76919951528</v>
+        <v>635.7114130810828</v>
       </c>
     </row>
     <row r="560">
       <c r="A560" t="n">
-        <v>581.0283203784365</v>
+        <v>611.1273958106267</v>
       </c>
     </row>
     <row r="561">
       <c r="A561" t="n">
-        <v>580.8380220889831</v>
+        <v>584.0285775300913</v>
       </c>
     </row>
     <row r="562">
       <c r="A562" t="n">
-        <v>609.6168868908194</v>
+        <v>599.3820538994328</v>
       </c>
     </row>
     <row r="563">
       <c r="A563" t="n">
-        <v>638.2444683605968</v>
+        <v>618.1421249632422</v>
       </c>
     </row>
     <row r="564">
       <c r="A564" t="n">
-        <v>646.1769579764223</v>
+        <v>640.9096067029623</v>
       </c>
     </row>
     <row r="565">
       <c r="A565" t="n">
-        <v>689.2451589931738</v>
+        <v>680.1276482567005</v>
       </c>
     </row>
     <row r="566">
       <c r="A566" t="n">
-        <v>638.557630459502</v>
+        <v>680.3887491967657</v>
       </c>
     </row>
     <row r="567">
       <c r="A567" t="n">
-        <v>589.8945619226197</v>
+        <v>635.7378502946176</v>
       </c>
     </row>
     <row r="568">
       <c r="A568" t="n">
-        <v>570.593301453016</v>
+        <v>561.2166303540107</v>
       </c>
     </row>
     <row r="569">
       <c r="A569" t="n">
-        <v>588.6739825848508</v>
+        <v>578.7937232778404</v>
       </c>
     </row>
     <row r="570">
       <c r="A570" t="n">
-        <v>566.2855496673842</v>
+        <v>593.1892717137544</v>
       </c>
     </row>
     <row r="571">
       <c r="A571" t="n">
-        <v>557.5498300159438</v>
+        <v>545.3949013224246</v>
       </c>
     </row>
     <row r="572">
       <c r="A572" t="n">
-        <v>599.8027716361776</v>
+        <v>588.767997545915</v>
       </c>
     </row>
     <row r="573">
       <c r="A573" t="n">
-        <v>613.9319968634709</v>
+        <v>619.0301257044553</v>
       </c>
     </row>
     <row r="574">
       <c r="A574" t="n">
-        <v>637.8935363401297</v>
+        <v>619.56753443053</v>
       </c>
     </row>
     <row r="575">
       <c r="A575" t="n">
-        <v>702.2167587968511</v>
+        <v>687.8576834080832</v>
       </c>
     </row>
     <row r="576">
       <c r="A576" t="n">
-        <v>683.7439081463117</v>
+        <v>699.5103294580645</v>
       </c>
     </row>
     <row r="577">
       <c r="A577" t="n">
-        <v>669.5530624500634</v>
+        <v>663.5091235235677</v>
       </c>
     </row>
     <row r="578">
       <c r="A578" t="n">
-        <v>614.1218054950173</v>
+        <v>643.9236684500997</v>
       </c>
     </row>
     <row r="579">
       <c r="A579" t="n">
-        <v>619.7198994890982</v>
+        <v>612.5531899679117</v>
       </c>
     </row>
     <row r="580">
       <c r="A580" t="n">
-        <v>680.4908603544959</v>
+        <v>661.9158289905727</v>
       </c>
     </row>
     <row r="581">
       <c r="A581" t="n">
-        <v>703.4270132248821</v>
+        <v>696.713845029592</v>
       </c>
     </row>
     <row r="582">
       <c r="A582" t="n">
-        <v>678.2341243754786</v>
+        <v>679.8003593802946</v>
       </c>
     </row>
     <row r="583">
       <c r="A583" t="n">
-        <v>722.9310323746745</v>
+        <v>708.826293570155</v>
       </c>
     </row>
     <row r="584">
       <c r="A584" t="n">
-        <v>684.3446780038107</v>
+        <v>710.1204081794776</v>
       </c>
     </row>
     <row r="585">
       <c r="A585" t="n">
-        <v>656.3310525122006</v>
+        <v>666.6851425134723</v>
       </c>
     </row>
     <row r="586">
       <c r="A586" t="n">
-        <v>638.0109593807219</v>
+        <v>644.1583688410333</v>
       </c>
     </row>
     <row r="587">
       <c r="A587" t="n">
-        <v>705.2265229543195</v>
+        <v>681.4882535566085</v>
       </c>
     </row>
     <row r="588">
       <c r="A588" t="n">
-        <v>706.8605208137342</v>
+        <v>701.069923476723</v>
       </c>
     </row>
     <row r="589">
       <c r="A589" t="n">
-        <v>670.3489780232417</v>
+        <v>697.7192555217471</v>
       </c>
     </row>
     <row r="590">
       <c r="A590" t="n">
-        <v>658.6327956429727</v>
+        <v>672.3520719700673</v>
       </c>
     </row>
     <row r="591">
       <c r="A591" t="n">
-        <v>654.2484845828085</v>
+        <v>636.792555440195</v>
       </c>
     </row>
     <row r="592">
       <c r="A592" t="n">
-        <v>619.1788054702556</v>
+        <v>625.0951878274691</v>
       </c>
     </row>
     <row r="593">
       <c r="A593" t="n">
-        <v>640.1920569598474</v>
+        <v>631.6203903920723</v>
       </c>
     </row>
     <row r="594">
       <c r="A594" t="n">
-        <v>600.8842003606674</v>
+        <v>616.88161057765</v>
       </c>
     </row>
     <row r="595">
       <c r="A595" t="n">
-        <v>619.0549917954513</v>
+        <v>603.7516625389685</v>
       </c>
     </row>
     <row r="596">
       <c r="A596" t="n">
-        <v>614.8935704159157</v>
+        <v>625.5064512318995</v>
       </c>
     </row>
     <row r="597">
       <c r="A597" t="n">
-        <v>598.4064811480607</v>
+        <v>604.610406164511</v>
       </c>
     </row>
     <row r="598">
       <c r="A598" t="n">
-        <v>655.9665679182558</v>
+        <v>626.8111150593541</v>
       </c>
     </row>
     <row r="599">
       <c r="A599" t="n">
-        <v>753.0931723296703</v>
+        <v>708.2548417924386</v>
       </c>
     </row>
     <row r="600">
       <c r="A600" t="n">
-        <v>724.3198356824792</v>
+        <v>751.7317297172212</v>
       </c>
     </row>
     <row r="601">
       <c r="A601" t="n">
-        <v>641.975547896493</v>
+        <v>693.3909917169103</v>
       </c>
     </row>
     <row r="602">
       <c r="A602" t="n">
-        <v>606.7393730451158</v>
+        <v>620.3958283814472</v>
       </c>
     </row>
     <row r="603">
       <c r="A603" t="n">
-        <v>592.0665449413605</v>
+        <v>606.8825366710371</v>
       </c>
     </row>
     <row r="604">
       <c r="A604" t="n">
-        <v>548.5635187804405</v>
+        <v>570.8419163123608</v>
       </c>
     </row>
     <row r="605">
       <c r="A605" t="n">
-        <v>482.9240405608743</v>
+        <v>514.695683178843</v>
       </c>
     </row>
     <row r="606">
       <c r="A606" t="n">
-        <v>470.3599609134699</v>
+        <v>476.195917868381</v>
       </c>
     </row>
     <row r="607">
       <c r="A607" t="n">
-        <v>483.8269330271032</v>
+        <v>477.6149814222208</v>
       </c>
     </row>
     <row r="608">
       <c r="A608" t="n">
-        <v>556.1643174860365</v>
+        <v>532.4523414478222</v>
       </c>
     </row>
     <row r="609">
       <c r="A609" t="n">
-        <v>633.3289981883468</v>
+        <v>605.1995243051351</v>
       </c>
     </row>
     <row r="610">
       <c r="A610" t="n">
-        <v>694.1140648366968</v>
+        <v>674.4311930427784</v>
       </c>
     </row>
     <row r="611">
       <c r="A611" t="n">
-        <v>715.81578185544</v>
+        <v>710.7346196808635</v>
       </c>
     </row>
     <row r="612">
       <c r="A612" t="n">
-        <v>695.3003202192463</v>
+        <v>730.7502832034629</v>
       </c>
     </row>
     <row r="613">
       <c r="A613" t="n">
-        <v>625.4338075265196</v>
+        <v>655.8288664049314</v>
       </c>
     </row>
     <row r="614">
       <c r="A614" t="n">
-        <v>530.9596988930707</v>
+        <v>552.9683948054185</v>
       </c>
     </row>
     <row r="615">
       <c r="A615" t="n">
-        <v>458.7956140474034</v>
+        <v>483.7595293588492</v>
       </c>
     </row>
     <row r="616">
       <c r="A616" t="n">
-        <v>429.8963948805294</v>
+        <v>455.360966959006</v>
       </c>
     </row>
     <row r="617">
       <c r="A617" t="n">
-        <v>420.7786608504307</v>
+        <v>417.4276012479936</v>
       </c>
     </row>
     <row r="618">
       <c r="A618" t="n">
-        <v>463.1404720062164</v>
+        <v>451.1353888595977</v>
       </c>
     </row>
     <row r="619">
       <c r="A619" t="n">
-        <v>493.5061550738737</v>
+        <v>480.3468601797363</v>
       </c>
     </row>
     <row r="620">
       <c r="A620" t="n">
-        <v>541.0339991012165</v>
+        <v>524.9994224209331</v>
       </c>
     </row>
     <row r="621">
       <c r="A621" t="n">
-        <v>553.0041600656546</v>
+        <v>562.4980652857516</v>
       </c>
     </row>
     <row r="622">
       <c r="A622" t="n">
-        <v>545.6856983514058</v>
+        <v>553.3825158607328</v>
       </c>
     </row>
     <row r="623">
       <c r="A623" t="n">
-        <v>551.8463656559334</v>
+        <v>541.6169082226361</v>
       </c>
     </row>
     <row r="624">
       <c r="A624" t="n">
-        <v>572.9175689620547</v>
+        <v>559.1701073656736</v>
       </c>
     </row>
     <row r="625">
       <c r="A625" t="n">
-        <v>522.1017895726732</v>
+        <v>540.0880227863922</v>
       </c>
     </row>
     <row r="626">
       <c r="A626" t="n">
-        <v>523.0934271720571</v>
+        <v>521.0080127096148</v>
       </c>
     </row>
     <row r="627">
       <c r="A627" t="n">
-        <v>498.7234928146904</v>
+        <v>503.5334747533398</v>
       </c>
     </row>
     <row r="628">
       <c r="A628" t="n">
-        <v>526.8365822567489</v>
+        <v>511.2090941995575</v>
       </c>
     </row>
     <row r="629">
       <c r="A629" t="n">
-        <v>543.5588418970383</v>
+        <v>539.2536094329898</v>
       </c>
     </row>
     <row r="630">
       <c r="A630" t="n">
-        <v>534.9770655927841</v>
+        <v>561.8178375921161</v>
       </c>
     </row>
     <row r="631">
       <c r="A631" t="n">
-        <v>517.9649917249662</v>
+        <v>513.2810932290113</v>
       </c>
     </row>
     <row r="632">
       <c r="A632" t="n">
-        <v>517.0168253229122</v>
+        <v>531.6344065218459</v>
       </c>
     </row>
     <row r="633">
       <c r="A633" t="n">
-        <v>513.6670905660026</v>
+        <v>508.0102098665407</v>
       </c>
     </row>
     <row r="634">
       <c r="A634" t="n">
-        <v>563.9062972618945</v>
+        <v>536.1164855119682</v>
       </c>
     </row>
     <row r="635">
       <c r="A635" t="n">
-        <v>635.6474088767641</v>
+        <v>617.0015387750141</v>
       </c>
     </row>
     <row r="636">
       <c r="A636" t="n">
-        <v>653.4963266004183</v>
+        <v>653.6820363068614</v>
       </c>
     </row>
     <row r="637">
       <c r="A637" t="n">
-        <v>647.4931212684396</v>
+        <v>643.9161908021447</v>
       </c>
     </row>
     <row r="638">
       <c r="A638" t="n">
-        <v>683.183943406334</v>
+        <v>666.2455514081671</v>
       </c>
     </row>
     <row r="639">
       <c r="A639" t="n">
-        <v>656.9262250872043</v>
+        <v>649.6267162233949</v>
       </c>
     </row>
     <row r="640">
       <c r="A640" t="n">
-        <v>641.876993011067</v>
+        <v>651.9613360420635</v>
       </c>
     </row>
     <row r="641">
       <c r="A641" t="n">
-        <v>607.2037925538893</v>
+        <v>611.0236893981096</v>
       </c>
     </row>
     <row r="642">
       <c r="A642" t="n">
-        <v>559.9196639457773</v>
+        <v>581.1615034228339</v>
       </c>
     </row>
     <row r="643">
       <c r="A643" t="n">
-        <v>488.4517232653707</v>
+        <v>496.5326571119704</v>
       </c>
     </row>
     <row r="644">
       <c r="A644" t="n">
-        <v>467.9677741623891</v>
+        <v>482.2163114108093</v>
       </c>
     </row>
     <row r="645">
       <c r="A645" t="n">
-        <v>488.5964745559477</v>
+        <v>486.2636213603082</v>
       </c>
     </row>
     <row r="646">
       <c r="A646" t="n">
-        <v>494.4296914298434</v>
+        <v>497.016181487254</v>
       </c>
     </row>
     <row r="647">
       <c r="A647" t="n">
-        <v>451.5714113373974</v>
+        <v>469.0328334246487</v>
       </c>
     </row>
     <row r="648">
       <c r="A648" t="n">
-        <v>483.6950061720131</v>
+        <v>464.6969889486172</v>
       </c>
     </row>
     <row r="649">
       <c r="A649" t="n">
-        <v>594.3861895225382</v>
+        <v>547.9892680166927</v>
       </c>
     </row>
     <row r="650">
       <c r="A650" t="n">
-        <v>653.9690275600947</v>
+        <v>640.8539036174261</v>
       </c>
     </row>
     <row r="651">
       <c r="A651" t="n">
-        <v>704.0781125737681</v>
+        <v>696.9788294542241</v>
       </c>
     </row>
     <row r="652">
       <c r="A652" t="n">
-        <v>694.2154597470562</v>
+        <v>702.5037441553081</v>
       </c>
     </row>
     <row r="653">
       <c r="A653" t="n">
-        <v>624.65209840542</v>
+        <v>649.8883153926158</v>
       </c>
     </row>
     <row r="654">
       <c r="A654" t="n">
-        <v>569.7407789808722</v>
+        <v>588.5846015626726</v>
       </c>
     </row>
     <row r="655">
       <c r="A655" t="n">
-        <v>560.9558007986379</v>
+        <v>571.9839217732101</v>
       </c>
     </row>
     <row r="656">
       <c r="A656" t="n">
-        <v>552.9684799344068</v>
+        <v>550.6490686208281</v>
       </c>
     </row>
     <row r="657">
       <c r="A657" t="n">
-        <v>522.1437428857598</v>
+        <v>537.417404804728</v>
       </c>
     </row>
     <row r="658">
       <c r="A658" t="n">
-        <v>510.4114215498612</v>
+        <v>514.4369310909838</v>
       </c>
     </row>
     <row r="659">
       <c r="A659" t="n">
-        <v>540.4715857606561</v>
+        <v>536.0976736952807</v>
       </c>
     </row>
     <row r="660">
       <c r="A660" t="n">
-        <v>596.4552110912678</v>
+        <v>567.7121665775644</v>
       </c>
     </row>
     <row r="661">
       <c r="A661" t="n">
-        <v>662.6942200238659</v>
+        <v>645.9428640774831</v>
       </c>
     </row>
     <row r="662">
       <c r="A662" t="n">
-        <v>674.9653779326081</v>
+        <v>696.6461516673235</v>
       </c>
     </row>
     <row r="663">
       <c r="A663" t="n">
-        <v>594.1828982728907</v>
+        <v>616.5470047885151</v>
       </c>
     </row>
     <row r="664">
       <c r="A664" t="n">
-        <v>531.9754822710365</v>
+        <v>549.8469026205726</v>
       </c>
     </row>
     <row r="665">
       <c r="A665" t="n">
-        <v>471.2341364578947</v>
+        <v>485.5717098265018</v>
       </c>
     </row>
     <row r="666">
       <c r="A666" t="n">
-        <v>442.2612254033993</v>
+        <v>440.2249203599808</v>
       </c>
     </row>
     <row r="667">
       <c r="A667" t="n">
-        <v>509.3884601590162</v>
+        <v>489.194765153627</v>
       </c>
     </row>
     <row r="668">
       <c r="A668" t="n">
-        <v>588.8612912076496</v>
+        <v>561.4221374731301</v>
       </c>
     </row>
     <row r="669">
       <c r="A669" t="n">
-        <v>658.8327021646592</v>
+        <v>645.0062691703806</v>
       </c>
     </row>
     <row r="670">
       <c r="A670" t="n">
-        <v>704.1158526486129</v>
+        <v>684.6306122871511</v>
       </c>
     </row>
     <row r="671">
       <c r="A671" t="n">
-        <v>685.3584643097861</v>
+        <v>717.8926156963712</v>
       </c>
     </row>
     <row r="672">
       <c r="A672" t="n">
-        <v>700.1973988112695</v>
+        <v>694.2295228845978</v>
       </c>
     </row>
     <row r="673">
       <c r="A673" t="n">
-        <v>713.368068035436</v>
+        <v>713.5079628478138</v>
       </c>
     </row>
     <row r="674">
       <c r="A674" t="n">
-        <v>703.9661265878863</v>
+        <v>708.0370285841013</v>
       </c>
     </row>
     <row r="675">
       <c r="A675" t="n">
-        <v>726.1862517682403</v>
+        <v>710.4122364685281</v>
       </c>
     </row>
     <row r="676">
       <c r="A676" t="n">
-        <v>736.9089829799123</v>
+        <v>737.7996606489319</v>
       </c>
     </row>
     <row r="677">
       <c r="A677" t="n">
-        <v>725.241926612739</v>
+        <v>733.3198003779557</v>
       </c>
     </row>
     <row r="678">
       <c r="A678" t="n">
-        <v>667.650632303264</v>
+        <v>675.1769744896023</v>
       </c>
     </row>
     <row r="679">
       <c r="A679" t="n">
-        <v>685.5911338492433</v>
+        <v>685.4397381816852</v>
       </c>
     </row>
     <row r="680">
       <c r="A680" t="n">
-        <v>712.3424349721859</v>
+        <v>706.7689917901703</v>
       </c>
     </row>
     <row r="681">
       <c r="A681" t="n">
-        <v>705.0710603264179</v>
+        <v>710.8788630394542</v>
       </c>
     </row>
     <row r="682">
       <c r="A682" t="n">
-        <v>682.6172668370987</v>
+        <v>663.5099903550099</v>
       </c>
     </row>
     <row r="683">
       <c r="A683" t="n">
-        <v>676.7419967396222</v>
+        <v>675.6074447730498</v>
       </c>
     </row>
     <row r="684">
       <c r="A684" t="n">
-        <v>611.4488477119266</v>
+        <v>624.73951128311</v>
       </c>
     </row>
     <row r="685">
       <c r="A685" t="n">
-        <v>604.7384139534984</v>
+        <v>614.9922233599341</v>
       </c>
     </row>
     <row r="686">
       <c r="A686" t="n">
-        <v>574.5453084378482</v>
+        <v>579.6956375151012</v>
       </c>
     </row>
     <row r="687">
       <c r="A687" t="n">
-        <v>563.960979223566</v>
+        <v>564.7906066278097</v>
       </c>
     </row>
     <row r="688">
       <c r="A688" t="n">
-        <v>582.2617532596723</v>
+        <v>581.953348097386</v>
       </c>
     </row>
     <row r="689">
       <c r="A689" t="n">
-        <v>591.0843618972876</v>
+        <v>575.3779207314551</v>
       </c>
     </row>
     <row r="690">
       <c r="A690" t="n">
-        <v>623.97221608569</v>
+        <v>623.079392143552</v>
       </c>
     </row>
     <row r="691">
       <c r="A691" t="n">
-        <v>635.5581876499627</v>
+        <v>624.5647838314312</v>
       </c>
     </row>
     <row r="692">
       <c r="A692" t="n">
-        <v>646.350858945425</v>
+        <v>626.7778916967472</v>
       </c>
     </row>
     <row r="693">
       <c r="A693" t="n">
-        <v>678.90241184557</v>
+        <v>660.5837073139469</v>
       </c>
     </row>
     <row r="694">
       <c r="A694" t="n">
-        <v>726.4484930657318</v>
+        <v>736.4312661609347</v>
       </c>
     </row>
     <row r="695">
       <c r="A695" t="n">
-        <v>741.8051662174889</v>
+        <v>736.4886836815572</v>
       </c>
     </row>
     <row r="696">
       <c r="A696" t="n">
-        <v>727.0152359724307</v>
+        <v>733.7853582317848</v>
       </c>
     </row>
     <row r="697">
       <c r="A697" t="n">
-        <v>669.4979953496727</v>
+        <v>679.9988719924954</v>
       </c>
     </row>
     <row r="698">
       <c r="A698" t="n">
-        <v>665.6894412117822</v>
+        <v>684.4096365119867</v>
       </c>
     </row>
     <row r="699">
       <c r="A699" t="n">
-        <v>608.3488287877685</v>
+        <v>618.3370521425218</v>
       </c>
     </row>
   </sheetData>

</xml_diff>